<commit_message>
many fixes and made pinout guide
</commit_message>
<xml_diff>
--- a/Instructions/Pinouts.xlsx
+++ b/Instructions/Pinouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen Cowen\Documents\GitHub\String_Pulling_System\Instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DB0CF5-8F85-4EE5-A1BE-DEF8B4FDAD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C1F611-DE87-4EBC-8A41-964A2921D0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31404" yWindow="2340" windowWidth="18852" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
   <si>
     <t>Panel Pinout</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Blue</t>
   </si>
   <si>
-    <t>To Acquistion System</t>
-  </si>
-  <si>
     <t>Rot Enc 1 Tic</t>
   </si>
   <si>
@@ -121,6 +118,114 @@
   </si>
   <si>
     <t>Could do short tics for CW and long tics for CCW so that only one line.</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>RotGND</t>
+  </si>
+  <si>
+    <t>Rot5V</t>
+  </si>
+  <si>
+    <t>Rot1TicA</t>
+  </si>
+  <si>
+    <t>Rot1TicB</t>
+  </si>
+  <si>
+    <t>Rot2TicA</t>
+  </si>
+  <si>
+    <t>Rot2TicB</t>
+  </si>
+  <si>
+    <t>Arduino Pin (0 based)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INPUT </t>
+  </si>
+  <si>
+    <t>Arduino 1 (Rotary Encoder Arduino)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTPUT </t>
+  </si>
+  <si>
+    <t>To Arduino 2 and Digital Out</t>
+  </si>
+  <si>
+    <t>Rot1CWTic</t>
+  </si>
+  <si>
+    <t>Rot1CCWTic</t>
+  </si>
+  <si>
+    <t>Rot2CWTic</t>
+  </si>
+  <si>
+    <t>Rot2CCWTic</t>
+  </si>
+  <si>
+    <t>Arduino 2 (Experiment Control Arduino)</t>
+  </si>
+  <si>
+    <t>Rot1_CW_Tic</t>
+  </si>
+  <si>
+    <t>Rot1_CCW_Tic</t>
+  </si>
+  <si>
+    <t>Rot2_CW_Tic</t>
+  </si>
+  <si>
+    <t>Rot2_CCW_Tic</t>
+  </si>
+  <si>
+    <t>General_IO1</t>
+  </si>
+  <si>
+    <t>General_IO2</t>
+  </si>
+  <si>
+    <t>Signal</t>
+  </si>
+  <si>
+    <t>Timing pulse</t>
+  </si>
+  <si>
+    <t>Feeder 1 triggered</t>
+  </si>
+  <si>
+    <t>Feeder 2 triggered</t>
+  </si>
+  <si>
+    <t>Sensor 1 tripped</t>
+  </si>
+  <si>
+    <t>Sensor 2 tripped</t>
+  </si>
+  <si>
+    <t>Sound 1 onset</t>
+  </si>
+  <si>
+    <t>Sound 2 onset</t>
+  </si>
+  <si>
+    <t>Pulses come in sets of 4 so 2^4 combos which should be enough</t>
+  </si>
+  <si>
+    <t>one pulse for each digital signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maze Event </t>
+  </si>
+  <si>
+    <t>External To Acquistion System</t>
+  </si>
+  <si>
+    <t>See the ppt - more clear I think</t>
   </si>
 </sst>
 </file>
@@ -439,28 +544,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="18.21875" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -473,6 +582,9 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
       <c r="G3">
         <v>1</v>
       </c>
@@ -493,17 +605,23 @@
       <c r="C4" t="s">
         <v>20</v>
       </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -516,11 +634,17 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -533,11 +657,17 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
       <c r="G6">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -550,11 +680,17 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
       <c r="G7">
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -562,10 +698,10 @@
         <v>6</v>
       </c>
       <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
         <v>29</v>
-      </c>
-      <c r="J8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -619,46 +755,257 @@
         <v>11</v>
       </c>
     </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17">
+        <v>8</v>
+      </c>
+      <c r="K17" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18">
+        <v>9</v>
+      </c>
+      <c r="K18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19">
+        <v>10</v>
+      </c>
+      <c r="K19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20">
+        <v>11</v>
+      </c>
+      <c r="K20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>38</v>
+      </c>
+      <c r="J29">
+        <v>14</v>
+      </c>
+      <c r="K29" t="s">
+        <v>52</v>
+      </c>
+      <c r="M29" t="s">
+        <v>54</v>
+      </c>
+      <c r="N29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>8</v>
+      </c>
+      <c r="H30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30">
+        <v>15</v>
+      </c>
+      <c r="K30" t="s">
+        <v>53</v>
+      </c>
+      <c r="M30" t="s">
+        <v>55</v>
+      </c>
+      <c r="N30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <v>9</v>
+      </c>
+      <c r="H31" t="s">
+        <v>49</v>
+      </c>
+      <c r="J31">
+        <v>16</v>
+      </c>
+      <c r="M31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <v>10</v>
+      </c>
+      <c r="H32" t="s">
+        <v>50</v>
+      </c>
+      <c r="J32">
+        <v>11</v>
+      </c>
+      <c r="K32" t="s">
+        <v>46</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <v>11</v>
+      </c>
+      <c r="H33" t="s">
+        <v>51</v>
+      </c>
+      <c r="M33">
+        <v>2</v>
+      </c>
+      <c r="N33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="M34">
+        <v>3</v>
+      </c>
+      <c r="N34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="M35">
+        <v>4</v>
+      </c>
+      <c r="N35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="M36">
+        <v>5</v>
+      </c>
+      <c r="N36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="M37">
+        <v>6</v>
+      </c>
+      <c r="N37" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>